<commit_message>
Updated validation reports to reflect current pipeline outputs
</commit_message>
<xml_diff>
--- a/cowbat/validation/reports/abundance_fasta.xlsx
+++ b/cowbat/validation/reports/abundance_fasta.xlsx
@@ -52,10 +52,10 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Escherichia</t>
   </si>
   <si>
-    <t>2649</t>
-  </si>
-  <si>
-    <t>99.9246</t>
+    <t>2644</t>
+  </si>
+  <si>
+    <t>99.9622</t>
   </si>
   <si>
     <t>100</t>
@@ -70,72 +70,69 @@
     <t>1639</t>
   </si>
   <si>
+    <t>Bacteria;Firmicutes;;Bacillales;;Listeria</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>2014-SEQ-0276</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>99.3056</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.694444</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2014-SEQ-0933</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>2014-SEQ-1049</t>
+  </si>
+  <si>
+    <t>Salmonella enterica</t>
+  </si>
+  <si>
+    <t>28901</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Salmonella</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>94.8276</t>
+  </si>
+  <si>
+    <t>98.2143</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3.44828</t>
+  </si>
+  <si>
     <t>Bacteria;Firmicutes;Bacilli;Bacillales;Listeriaceae;Listeria</t>
   </si>
   <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>99.5851</t>
-  </si>
-  <si>
-    <t>2014-SEQ-0276</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>99.3056</t>
-  </si>
-  <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.694444</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>2014-SEQ-0933</t>
-  </si>
-  <si>
-    <t>Bacteria;Firmicutes;;Bacillales;;Listeria</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>2014-SEQ-1049</t>
-  </si>
-  <si>
-    <t>Salmonella enterica</t>
-  </si>
-  <si>
-    <t>28901</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Salmonella</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>94.8276</t>
-  </si>
-  <si>
-    <t>98.2143</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3.44828</t>
-  </si>
-  <si>
     <t>1.72414</t>
   </si>
   <si>
@@ -145,13 +142,13 @@
     <t>2015-SEQ-0423</t>
   </si>
   <si>
-    <t>2754</t>
-  </si>
-  <si>
-    <t>99.4224</t>
-  </si>
-  <si>
-    <t>99.4942</t>
+    <t>2758</t>
+  </si>
+  <si>
+    <t>99.4232</t>
+  </si>
+  <si>
+    <t>99.4949</t>
   </si>
   <si>
     <t>2015-SEQ-0626</t>
@@ -262,13 +259,13 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Proteus</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>43.75</t>
-  </si>
-  <si>
-    <t>48.8372</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>44.898</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
   <si>
     <t>Providencia stuartii</t>
@@ -283,295 +280,298 @@
     <t>5</t>
   </si>
   <si>
-    <t>10.4167</t>
-  </si>
-  <si>
-    <t>11.6279</t>
+    <t>10.2041</t>
+  </si>
+  <si>
+    <t>11.3636</t>
+  </si>
+  <si>
+    <t>4.08163</t>
+  </si>
+  <si>
+    <t>4.54545</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>573</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Klebsiella</t>
+  </si>
+  <si>
+    <t>Morganella morganii</t>
+  </si>
+  <si>
+    <t>582</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Morganella</t>
+  </si>
+  <si>
+    <t>Providencia rustigianii</t>
+  </si>
+  <si>
+    <t>158850</t>
+  </si>
+  <si>
+    <t>Arsenophonus nasoniae</t>
+  </si>
+  <si>
+    <t>638</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Arsenophonus</t>
+  </si>
+  <si>
+    <t>2.04082</t>
+  </si>
+  <si>
+    <t>2.27273</t>
+  </si>
+  <si>
+    <t>Burkholderia pseudomallei</t>
+  </si>
+  <si>
+    <t>28450</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Betaproteobacteria;Burkholderiales;Burkholderiaceae;Burkholderia</t>
+  </si>
+  <si>
+    <t>Haemophilus influenzae</t>
+  </si>
+  <si>
+    <t>727</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pasteurellales;Pasteurellaceae;Haemophilus</t>
+  </si>
+  <si>
+    <t>Providencia rettgeri</t>
+  </si>
+  <si>
+    <t>587</t>
+  </si>
+  <si>
+    <t>Pseudoalteromonas agarivorans</t>
+  </si>
+  <si>
+    <t>176102</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Alteromonadales;Pseudoalteromonadaceae;Pseudoalteromonas</t>
+  </si>
+  <si>
+    <t>Shigella dysenteriae</t>
+  </si>
+  <si>
+    <t>622</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Shigella</t>
+  </si>
+  <si>
+    <t>Yersinia pestis</t>
+  </si>
+  <si>
+    <t>632</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Yersiniaceae;Yersinia</t>
+  </si>
+  <si>
+    <t>2017-HCLON-0380</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>97.4249</t>
+  </si>
+  <si>
+    <t>99.1266</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1.71674</t>
+  </si>
+  <si>
+    <t>2017-SEQ-0905</t>
+  </si>
+  <si>
+    <t>Acinetobacter baumannii</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>94.0541</t>
+  </si>
+  <si>
+    <t>95.6044</t>
+  </si>
+  <si>
+    <t>Acinetobacter calcoaceticus</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>2.16216</t>
+  </si>
+  <si>
+    <t>2.1978</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1.62162</t>
+  </si>
+  <si>
+    <t>Acinetobacter nosocomialis</t>
+  </si>
+  <si>
+    <t>106654</t>
+  </si>
+  <si>
+    <t>1.08108</t>
+  </si>
+  <si>
+    <t>1.0989</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii</t>
+  </si>
+  <si>
+    <t>48296</t>
+  </si>
+  <si>
+    <t>2017-SEQ-1501</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>96.6667</t>
+  </si>
+  <si>
+    <t>Enterococcus faecium</t>
+  </si>
+  <si>
+    <t>1352</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;;;;Enterococcus</t>
+  </si>
+  <si>
+    <t>3.33333</t>
+  </si>
+  <si>
+    <t>2018-STH-0076</t>
+  </si>
+  <si>
+    <t>2016-SEQ-1221</t>
+  </si>
+  <si>
+    <t>Enterobacter hormaechei</t>
+  </si>
+  <si>
+    <t>158836</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Enterobacter</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>19.4444</t>
+  </si>
+  <si>
+    <t>20.8955</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>18.0556</t>
+  </si>
+  <si>
+    <t>19.403</t>
+  </si>
+  <si>
+    <t>Enterobacter cloacae</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>13.4328</t>
+  </si>
+  <si>
+    <t>Enterobacter asburiae</t>
+  </si>
+  <si>
+    <t>61645</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>11.1111</t>
+  </si>
+  <si>
+    <t>11.9403</t>
+  </si>
+  <si>
+    <t>8.33333</t>
+  </si>
+  <si>
+    <t>8.95522</t>
+  </si>
+  <si>
+    <t>Enterobacter roggenkampii</t>
+  </si>
+  <si>
+    <t>1812935</t>
+  </si>
+  <si>
+    <t>6.94444</t>
+  </si>
+  <si>
+    <t>7.46269</t>
+  </si>
+  <si>
+    <t>5.55556</t>
+  </si>
+  <si>
+    <t>5.97015</t>
+  </si>
+  <si>
+    <t>Enterobacter sp. HK169</t>
+  </si>
+  <si>
+    <t>1868135</t>
   </si>
   <si>
     <t>4.16667</t>
-  </si>
-  <si>
-    <t>4.65116</t>
-  </si>
-  <si>
-    <t>Klebsiella pneumoniae</t>
-  </si>
-  <si>
-    <t>573</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Klebsiella</t>
-  </si>
-  <si>
-    <t>Morganella morganii</t>
-  </si>
-  <si>
-    <t>582</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Morganella</t>
-  </si>
-  <si>
-    <t>Providencia rustigianii</t>
-  </si>
-  <si>
-    <t>158850</t>
-  </si>
-  <si>
-    <t>Arsenophonus nasoniae</t>
-  </si>
-  <si>
-    <t>638</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Arsenophonus</t>
-  </si>
-  <si>
-    <t>2.08333</t>
-  </si>
-  <si>
-    <t>2.32558</t>
-  </si>
-  <si>
-    <t>Burkholderia pseudomallei</t>
-  </si>
-  <si>
-    <t>28450</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Betaproteobacteria;Burkholderiales;Burkholderiaceae;Burkholderia</t>
-  </si>
-  <si>
-    <t>Haemophilus influenzae</t>
-  </si>
-  <si>
-    <t>727</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pasteurellales;Pasteurellaceae;Haemophilus</t>
-  </si>
-  <si>
-    <t>Providencia rettgeri</t>
-  </si>
-  <si>
-    <t>587</t>
-  </si>
-  <si>
-    <t>Pseudoalteromonas agarivorans</t>
-  </si>
-  <si>
-    <t>176102</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Alteromonadales;Pseudoalteromonadaceae;Pseudoalteromonas</t>
-  </si>
-  <si>
-    <t>Shigella dysenteriae</t>
-  </si>
-  <si>
-    <t>622</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Shigella</t>
-  </si>
-  <si>
-    <t>Yersinia pestis</t>
-  </si>
-  <si>
-    <t>632</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Yersiniaceae;Yersinia</t>
-  </si>
-  <si>
-    <t>2017-HCLON-0380</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>97.4249</t>
-  </si>
-  <si>
-    <t>99.1266</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1.71674</t>
-  </si>
-  <si>
-    <t>2017-SEQ-0905</t>
-  </si>
-  <si>
-    <t>Acinetobacter baumannii</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter</t>
-  </si>
-  <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>94.0541</t>
-  </si>
-  <si>
-    <t>95.6044</t>
-  </si>
-  <si>
-    <t>Acinetobacter calcoaceticus</t>
-  </si>
-  <si>
-    <t>471</t>
-  </si>
-  <si>
-    <t>2.16216</t>
-  </si>
-  <si>
-    <t>2.1978</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1.62162</t>
-  </si>
-  <si>
-    <t>Acinetobacter nosocomialis</t>
-  </si>
-  <si>
-    <t>106654</t>
-  </si>
-  <si>
-    <t>1.08108</t>
-  </si>
-  <si>
-    <t>1.0989</t>
-  </si>
-  <si>
-    <t>Acinetobacter pittii</t>
-  </si>
-  <si>
-    <t>48296</t>
-  </si>
-  <si>
-    <t>2017-SEQ-1501</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>96.6667</t>
-  </si>
-  <si>
-    <t>Enterococcus faecium</t>
-  </si>
-  <si>
-    <t>1352</t>
-  </si>
-  <si>
-    <t>Bacteria;Firmicutes;;;;Enterococcus</t>
-  </si>
-  <si>
-    <t>3.33333</t>
-  </si>
-  <si>
-    <t>2018-STH-0076</t>
-  </si>
-  <si>
-    <t>2016-SEQ-1221</t>
-  </si>
-  <si>
-    <t>Enterobacter hormaechei</t>
-  </si>
-  <si>
-    <t>158836</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Enterobacter</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>19.4444</t>
-  </si>
-  <si>
-    <t>20.8955</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>18.0556</t>
-  </si>
-  <si>
-    <t>19.403</t>
-  </si>
-  <si>
-    <t>Enterobacter cloacae</t>
-  </si>
-  <si>
-    <t>550</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>13.4328</t>
-  </si>
-  <si>
-    <t>Enterobacter asburiae</t>
-  </si>
-  <si>
-    <t>61645</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>11.1111</t>
-  </si>
-  <si>
-    <t>11.9403</t>
-  </si>
-  <si>
-    <t>8.33333</t>
-  </si>
-  <si>
-    <t>8.95522</t>
-  </si>
-  <si>
-    <t>Enterobacter roggenkampii</t>
-  </si>
-  <si>
-    <t>1812935</t>
-  </si>
-  <si>
-    <t>6.94444</t>
-  </si>
-  <si>
-    <t>7.46269</t>
-  </si>
-  <si>
-    <t>5.55556</t>
-  </si>
-  <si>
-    <t>5.97015</t>
-  </si>
-  <si>
-    <t>Enterobacter sp. HK169</t>
-  </si>
-  <si>
-    <t>1868135</t>
   </si>
   <si>
     <t>4.47761</t>
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>4805065</v>
+        <v>4799130</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -1175,13 +1175,13 @@
         <v>18</v>
       </c>
       <c r="E3" s="2">
-        <v>2987345</v>
+        <v>2987342</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -1204,10 +1204,10 @@
         <v>5371470</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
@@ -1215,30 +1215,30 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -1247,13 +1247,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
         <v>3051674</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -1264,51 +1264,51 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="2">
         <v>4716660</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1319,304 +1319,304 @@
         <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2">
         <v>485</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3999918</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3996367</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="2">
         <v>5096300</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2">
         <v>1097202</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>23345</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="2">
         <v>141568</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2">
         <v>926</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="2">
         <v>2045</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2">
         <v>912</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2">
+        <v>2789846</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="2">
-        <v>2790142</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="B20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E20" s="2">
         <v>179487</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="H21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1633,271 +1633,271 @@
         <v>49540</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="E23" s="2">
         <v>209484</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="E24" s="2">
         <v>8646</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="2">
         <v>18392</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E26" s="2">
         <v>10158</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E27" s="2">
         <v>58416</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="E28" s="2">
         <v>24890</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E29" s="2">
         <v>610</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30" s="2">
         <v>1785</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E31" s="2">
         <v>52660</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="B32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E32" s="2">
         <v>6930</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="B33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="E33" s="2">
         <v>8447</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -1909,162 +1909,162 @@
         <v>11</v>
       </c>
       <c r="E34" s="2">
-        <v>5288199</v>
+        <v>5288123</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2">
+        <v>3919029</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E36" s="2">
-        <v>3918966</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="B37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37" s="2">
         <v>4431</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="B38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="2">
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="B39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E39" s="2">
         <v>3289</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="B40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E40" s="2">
         <v>3892</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>16</v>
@@ -2073,211 +2073,211 @@
         <v>17</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E41" s="2">
         <v>3016528</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E42" s="2">
         <v>754</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="E44" s="2">
         <v>1902398</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="B45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="E45" s="2">
         <v>64323</v>
       </c>
       <c r="F45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="B46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E46" s="2">
         <v>354449</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="B47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E47" s="2">
         <v>1850469</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="B48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E48" s="2">
         <v>78305</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E49" s="2">
         <v>3125</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2294,33 +2294,33 @@
         <v>189432</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E52" s="2">
         <v>9189</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>91</v>
+        <v>185</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>186</v>
@@ -2334,13 +2334,13 @@
         <v>188</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E53" s="2">
         <v>201160</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>189</v>
@@ -2357,13 +2357,13 @@
         <v>192</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E54" s="2">
         <v>1803</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>189</v>
@@ -2380,13 +2380,13 @@
         <v>194</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E55" s="2">
         <v>232</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>189</v>
@@ -2409,7 +2409,7 @@
         <v>540</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>189</v>
@@ -2420,19 +2420,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="B57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="E57" s="2">
         <v>86325</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>189</v>
@@ -2455,7 +2455,7 @@
         <v>201</v>
       </c>
       <c r="E58" s="2">
-        <v>5094684</v>
+        <v>5094020</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>202</v>
@@ -2469,25 +2469,25 @@
     </row>
     <row r="59" spans="1:8">
       <c r="B59" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>205</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2504,7 +2504,7 @@
         <v>16154</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>208</v>
@@ -2527,7 +2527,7 @@
         <v>213</v>
       </c>
       <c r="E61" s="2">
-        <v>1715084</v>
+        <v>1715091</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>214</v>
@@ -2553,7 +2553,7 @@
         <v>12591</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>218</v>
@@ -2625,7 +2625,7 @@
         <v>68844</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>233</v>
@@ -2673,13 +2673,13 @@
         <v>17</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E68" s="2">
         <v>2983937</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>240</v>
@@ -2690,19 +2690,19 @@
     </row>
     <row r="69" spans="1:8">
       <c r="B69" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="E69" s="2">
         <v>3326</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Added quast to pipeline
</commit_message>
<xml_diff>
--- a/cowbat/validation/reports/abundance_fasta.xlsx
+++ b/cowbat/validation/reports/abundance_fasta.xlsx
@@ -52,10 +52,10 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Escherichia</t>
   </si>
   <si>
-    <t>2644</t>
-  </si>
-  <si>
-    <t>99.9622</t>
+    <t>2634</t>
+  </si>
+  <si>
+    <t>99.962</t>
   </si>
   <si>
     <t>100</t>
@@ -142,13 +142,13 @@
     <t>2015-SEQ-0423</t>
   </si>
   <si>
-    <t>2758</t>
-  </si>
-  <si>
-    <t>99.4232</t>
-  </si>
-  <si>
-    <t>99.4949</t>
+    <t>2764</t>
+  </si>
+  <si>
+    <t>99.4245</t>
+  </si>
+  <si>
+    <t>99.496</t>
   </si>
   <si>
     <t>2015-SEQ-0626</t>
@@ -385,19 +385,19 @@
     <t>2017-HCLON-0380</t>
   </si>
   <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>97.4249</t>
-  </si>
-  <si>
-    <t>99.1266</t>
+    <t>223</t>
+  </si>
+  <si>
+    <t>97.3799</t>
+  </si>
+  <si>
+    <t>99.1111</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>1.71674</t>
+    <t>1.74672</t>
   </si>
   <si>
     <t>2017-SEQ-0905</t>
@@ -412,13 +412,13 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter</t>
   </si>
   <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>94.0541</t>
-  </si>
-  <si>
-    <t>95.6044</t>
+    <t>176</t>
+  </si>
+  <si>
+    <t>94.1176</t>
+  </si>
+  <si>
+    <t>95.6522</t>
   </si>
   <si>
     <t>Acinetobacter calcoaceticus</t>
@@ -427,16 +427,16 @@
     <t>471</t>
   </si>
   <si>
-    <t>2.16216</t>
-  </si>
-  <si>
-    <t>2.1978</t>
+    <t>2.13904</t>
+  </si>
+  <si>
+    <t>2.17391</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>1.62162</t>
+    <t>1.60428</t>
   </si>
   <si>
     <t>Acinetobacter nosocomialis</t>
@@ -445,10 +445,10 @@
     <t>106654</t>
   </si>
   <si>
-    <t>1.08108</t>
-  </si>
-  <si>
-    <t>1.0989</t>
+    <t>1.06952</t>
+  </si>
+  <si>
+    <t>1.08696</t>
   </si>
   <si>
     <t>Acinetobacter pittii</t>
@@ -730,22 +730,22 @@
     <t>203</t>
   </si>
   <si>
-    <t>84.9372</t>
-  </si>
-  <si>
     <t>85.2941</t>
   </si>
   <si>
-    <t>12.1339</t>
+    <t>85.654</t>
   </si>
   <si>
     <t>12.1849</t>
   </si>
   <si>
-    <t>1.25523</t>
-  </si>
-  <si>
-    <t>1.2605</t>
+    <t>12.2363</t>
+  </si>
+  <si>
+    <t>0.840336</t>
+  </si>
+  <si>
+    <t>0.843882</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>4799130</v>
+        <v>4793471</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -1348,7 +1348,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="2">
-        <v>3999918</v>
+        <v>4001831</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -1909,7 +1909,7 @@
         <v>11</v>
       </c>
       <c r="E34" s="2">
-        <v>5288123</v>
+        <v>5288405</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>123</v>
@@ -1958,7 +1958,7 @@
         <v>131</v>
       </c>
       <c r="E36" s="2">
-        <v>3919029</v>
+        <v>3918535</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>132</v>
@@ -2455,7 +2455,7 @@
         <v>201</v>
       </c>
       <c r="E58" s="2">
-        <v>5094020</v>
+        <v>5094690</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>202</v>
@@ -2653,7 +2653,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="2">
-        <v>692141</v>
+        <v>694771</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>237</v>
@@ -2676,7 +2676,7 @@
         <v>38</v>
       </c>
       <c r="E68" s="2">
-        <v>2983937</v>
+        <v>2983949</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>148</v>
@@ -2699,10 +2699,10 @@
         <v>80</v>
       </c>
       <c r="E69" s="2">
-        <v>3326</v>
+        <v>3550</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Update to validation reports to reflect new columns
</commit_message>
<xml_diff>
--- a/cowbat/validation/reports/abundance_fasta.xlsx
+++ b/cowbat/validation/reports/abundance_fasta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="243">
   <si>
     <t>Strain</t>
   </si>
@@ -52,10 +52,10 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Escherichia</t>
   </si>
   <si>
-    <t>2634</t>
-  </si>
-  <si>
-    <t>99.962</t>
+    <t>2655</t>
+  </si>
+  <si>
+    <t>99.9247</t>
   </si>
   <si>
     <t>100</t>
@@ -115,637 +115,634 @@
     <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Salmonella</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>94.8276</t>
-  </si>
-  <si>
-    <t>98.2143</t>
+    <t>54</t>
+  </si>
+  <si>
+    <t>94.7368</t>
+  </si>
+  <si>
+    <t>98.1818</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
+    <t>3.50877</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Listeriaceae;Listeria</t>
+  </si>
+  <si>
+    <t>1.75439</t>
+  </si>
+  <si>
+    <t>1.81818</t>
+  </si>
+  <si>
+    <t>2015-SEQ-0423</t>
+  </si>
+  <si>
+    <t>2769</t>
+  </si>
+  <si>
+    <t>99.3898</t>
+  </si>
+  <si>
+    <t>99.4612</t>
+  </si>
+  <si>
+    <t>2015-SEQ-0626</t>
+  </si>
+  <si>
+    <t>Pseudomonas fluorescens</t>
+  </si>
+  <si>
+    <t>294</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Pseudomonadaceae;Pseudomonas</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>61.4035</t>
+  </si>
+  <si>
+    <t>61.9469</t>
+  </si>
+  <si>
+    <t>Pseudomonas chlororaphis</t>
+  </si>
+  <si>
+    <t>587753</t>
+  </si>
+  <si>
+    <t>20.1754</t>
+  </si>
+  <si>
+    <t>20.354</t>
+  </si>
+  <si>
+    <t>Pseudomonas sp. S150</t>
+  </si>
+  <si>
+    <t>2559074</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>12.2807</t>
+  </si>
+  <si>
+    <t>12.3894</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>1.76991</t>
+  </si>
+  <si>
+    <t>Pseudomonas sp. RU47</t>
+  </si>
+  <si>
+    <t>2005388</t>
+  </si>
+  <si>
+    <t>Pseudomonas koreensis</t>
+  </si>
+  <si>
+    <t>198620</t>
+  </si>
+  <si>
+    <t>0.877193</t>
+  </si>
+  <si>
+    <t>0.884956</t>
+  </si>
+  <si>
+    <t>Pseudomonas syringae</t>
+  </si>
+  <si>
+    <t>317</t>
+  </si>
+  <si>
+    <t>2015-SEQ-1361</t>
+  </si>
+  <si>
+    <t>Proteus mirabilis</t>
+  </si>
+  <si>
+    <t>584</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Proteus</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>39.5833</t>
+  </si>
+  <si>
+    <t>43.1818</t>
+  </si>
+  <si>
+    <t>Providencia stuartii</t>
+  </si>
+  <si>
+    <t>588</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Providencia</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>14.5833</t>
+  </si>
+  <si>
+    <t>15.9091</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8.33333</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6.25</t>
+  </si>
+  <si>
+    <t>6.81818</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>573</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Klebsiella</t>
+  </si>
+  <si>
+    <t>4.16667</t>
+  </si>
+  <si>
+    <t>4.54545</t>
+  </si>
+  <si>
+    <t>Morganella morganii</t>
+  </si>
+  <si>
+    <t>582</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Morganella</t>
+  </si>
+  <si>
+    <t>Providencia rettgeri</t>
+  </si>
+  <si>
+    <t>587</t>
+  </si>
+  <si>
+    <t>Arsenophonus nasoniae</t>
+  </si>
+  <si>
+    <t>638</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Arsenophonus</t>
+  </si>
+  <si>
+    <t>2.08333</t>
+  </si>
+  <si>
+    <t>2.27273</t>
+  </si>
+  <si>
+    <t>Burkholderia pseudomallei</t>
+  </si>
+  <si>
+    <t>28450</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Betaproteobacteria;Burkholderiales;Burkholderiaceae;Burkholderia</t>
+  </si>
+  <si>
+    <t>Haemophilus influenzae</t>
+  </si>
+  <si>
+    <t>727</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pasteurellales;Pasteurellaceae;Haemophilus</t>
+  </si>
+  <si>
+    <t>Providencia rustigianii</t>
+  </si>
+  <si>
+    <t>158850</t>
+  </si>
+  <si>
+    <t>Pseudoalteromonas agarivorans</t>
+  </si>
+  <si>
+    <t>176102</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Alteromonadales;Pseudoalteromonadaceae;Pseudoalteromonas</t>
+  </si>
+  <si>
+    <t>Shigella sonnei</t>
+  </si>
+  <si>
+    <t>624</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Shigella</t>
+  </si>
+  <si>
+    <t>Yersinia pestis</t>
+  </si>
+  <si>
+    <t>632</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Yersiniaceae;Yersinia</t>
+  </si>
+  <si>
+    <t>Yersinia pseudotuberculosis</t>
+  </si>
+  <si>
+    <t>633</t>
+  </si>
+  <si>
+    <t>2017-HCLON-0380</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>96.9957</t>
+  </si>
+  <si>
+    <t>99.1228</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2.14592</t>
+  </si>
+  <si>
+    <t>2017-SEQ-0905</t>
+  </si>
+  <si>
+    <t>Acinetobacter baumannii</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>94.5946</t>
+  </si>
+  <si>
+    <t>96.1538</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii</t>
+  </si>
+  <si>
+    <t>48296</t>
+  </si>
+  <si>
+    <t>2.16216</t>
+  </si>
+  <si>
+    <t>2.1978</t>
+  </si>
+  <si>
+    <t>Acinetobacter nosocomialis</t>
+  </si>
+  <si>
+    <t>106654</t>
+  </si>
+  <si>
+    <t>1.62162</t>
+  </si>
+  <si>
+    <t>1.64835</t>
+  </si>
+  <si>
+    <t>2017-SEQ-1501</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>96.6667</t>
+  </si>
+  <si>
+    <t>Enterococcus faecium</t>
+  </si>
+  <si>
+    <t>1352</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;;;;Enterococcus</t>
+  </si>
+  <si>
+    <t>3.33333</t>
+  </si>
+  <si>
+    <t>2016-SEQ-1221</t>
+  </si>
+  <si>
+    <t>Enterobacter asburiae</t>
+  </si>
+  <si>
+    <t>61645</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Enterobacter</t>
+  </si>
+  <si>
+    <t>31.9444</t>
+  </si>
+  <si>
+    <t>34.3284</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>20.8333</t>
+  </si>
+  <si>
+    <t>22.3881</t>
+  </si>
+  <si>
+    <t>Enterobacter hormaechei</t>
+  </si>
+  <si>
+    <t>158836</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>11.1111</t>
+  </si>
+  <si>
+    <t>11.9403</t>
+  </si>
+  <si>
+    <t>Enterobacter cloacae</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>6.94444</t>
+  </si>
+  <si>
+    <t>7.46269</t>
+  </si>
+  <si>
+    <t>Enterobacter roggenkampii</t>
+  </si>
+  <si>
+    <t>1812935</t>
+  </si>
+  <si>
+    <t>5.55556</t>
+  </si>
+  <si>
+    <t>5.97015</t>
+  </si>
+  <si>
+    <t>Enterobacter ludwigii</t>
+  </si>
+  <si>
+    <t>299767</t>
+  </si>
+  <si>
+    <t>1.38889</t>
+  </si>
+  <si>
+    <t>1.49254</t>
+  </si>
+  <si>
+    <t>Enterobacter sp. 18A13</t>
+  </si>
+  <si>
+    <t>2565914</t>
+  </si>
+  <si>
+    <t>Klebsiella aerogenes</t>
+  </si>
+  <si>
+    <t>548</t>
+  </si>
+  <si>
+    <t>2018-SEQ-0843</t>
+  </si>
+  <si>
+    <t>Vibrio parahaemolyticus</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Vibrionales;Vibrionaceae;Vibrio</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>95.1613</t>
+  </si>
+  <si>
+    <t>98.3333</t>
+  </si>
+  <si>
+    <t>3.22581</t>
+  </si>
+  <si>
+    <t>Vibrio anguillarum</t>
+  </si>
+  <si>
+    <t>55601</t>
+  </si>
+  <si>
+    <t>1.6129</t>
+  </si>
+  <si>
+    <t>1.66667</t>
+  </si>
+  <si>
+    <t>2018-LET-0007</t>
+  </si>
+  <si>
+    <t>Campylobacter jejuni</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>Bacteria;;;;;Campylobacter</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>2018-STH-0255</t>
+  </si>
+  <si>
+    <t>Bacillus cereus</t>
+  </si>
+  <si>
+    <t>1396</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Bacillaceae;Bacillus</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>63.3333</t>
+  </si>
+  <si>
+    <t>63.6364</t>
+  </si>
+  <si>
+    <t>Bacillus anthracis</t>
+  </si>
+  <si>
+    <t>1392</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>34.2857</t>
+  </si>
+  <si>
+    <t>34.4498</t>
+  </si>
+  <si>
+    <t>Bacillus thuringiensis</t>
+  </si>
+  <si>
+    <t>1428</t>
+  </si>
+  <si>
+    <t>1.90476</t>
+  </si>
+  <si>
+    <t>1.91388</t>
+  </si>
+  <si>
+    <t>2014-SEQ-0335</t>
+  </si>
+  <si>
+    <t>2019-SEQ-0183</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>84.9372</t>
+  </si>
+  <si>
+    <t>85.2941</t>
+  </si>
+  <si>
+    <t>12.1339</t>
+  </si>
+  <si>
+    <t>12.1849</t>
+  </si>
+  <si>
+    <t>1.25523</t>
+  </si>
+  <si>
+    <t>1.2605</t>
+  </si>
+  <si>
+    <t>NC_003198_NC_003197_0_1_50_HS25</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;;Enterobacteriaceae;Salmonella</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96.9388</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;;Enterobacteriaceae;Escherichia</t>
+  </si>
+  <si>
+    <t>3.06122</t>
+  </si>
+  <si>
+    <t>2019-CAL-0091</t>
+  </si>
+  <si>
+    <t>Cronobacter sakazakii</t>
+  </si>
+  <si>
+    <t>28141</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Cronobacter</t>
+  </si>
+  <si>
+    <t>65.5172</t>
+  </si>
+  <si>
+    <t>16.6667</t>
+  </si>
+  <si>
+    <t>17.2414</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10.3448</t>
+  </si>
+  <si>
     <t>3.44828</t>
   </si>
   <si>
-    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Listeriaceae;Listeria</t>
-  </si>
-  <si>
-    <t>1.72414</t>
-  </si>
-  <si>
-    <t>1.78571</t>
-  </si>
-  <si>
-    <t>2015-SEQ-0423</t>
-  </si>
-  <si>
-    <t>2764</t>
-  </si>
-  <si>
-    <t>99.4245</t>
-  </si>
-  <si>
-    <t>99.496</t>
-  </si>
-  <si>
-    <t>2015-SEQ-0626</t>
-  </si>
-  <si>
-    <t>Pseudomonas fluorescens</t>
-  </si>
-  <si>
-    <t>294</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Pseudomonadaceae;Pseudomonas</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>62.2807</t>
-  </si>
-  <si>
-    <t>62.8319</t>
-  </si>
-  <si>
-    <t>Pseudomonas chlororaphis</t>
-  </si>
-  <si>
-    <t>587753</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>17.5439</t>
-  </si>
-  <si>
-    <t>17.6991</t>
-  </si>
-  <si>
-    <t>Pseudomonas sp. S150</t>
-  </si>
-  <si>
-    <t>2559074</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10.5263</t>
-  </si>
-  <si>
-    <t>10.6195</t>
-  </si>
-  <si>
-    <t>Pseudomonas koreensis</t>
-  </si>
-  <si>
-    <t>198620</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5.26316</t>
-  </si>
-  <si>
-    <t>5.30973</t>
-  </si>
-  <si>
-    <t>Pseudomonas aeruginosa</t>
-  </si>
-  <si>
-    <t>287</t>
-  </si>
-  <si>
-    <t>1.75439</t>
-  </si>
-  <si>
-    <t>1.76991</t>
-  </si>
-  <si>
-    <t>Pseudomonas sp. RU47</t>
-  </si>
-  <si>
-    <t>2005388</t>
-  </si>
-  <si>
-    <t>0.877193</t>
-  </si>
-  <si>
-    <t>0.884956</t>
-  </si>
-  <si>
-    <t>Pseudomonas syringae</t>
-  </si>
-  <si>
-    <t>317</t>
-  </si>
-  <si>
-    <t>2015-SEQ-1361</t>
-  </si>
-  <si>
-    <t>Proteus mirabilis</t>
-  </si>
-  <si>
-    <t>584</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Proteus</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>44.898</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Providencia stuartii</t>
-  </si>
-  <si>
-    <t>588</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Providencia</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>10.2041</t>
-  </si>
-  <si>
-    <t>11.3636</t>
-  </si>
-  <si>
-    <t>4.08163</t>
-  </si>
-  <si>
-    <t>4.54545</t>
-  </si>
-  <si>
-    <t>Klebsiella pneumoniae</t>
-  </si>
-  <si>
-    <t>573</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Klebsiella</t>
-  </si>
-  <si>
-    <t>Morganella morganii</t>
-  </si>
-  <si>
-    <t>582</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Morganella</t>
-  </si>
-  <si>
-    <t>Providencia rustigianii</t>
-  </si>
-  <si>
-    <t>158850</t>
-  </si>
-  <si>
-    <t>Arsenophonus nasoniae</t>
-  </si>
-  <si>
-    <t>638</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Arsenophonus</t>
-  </si>
-  <si>
-    <t>2.04082</t>
-  </si>
-  <si>
-    <t>2.27273</t>
-  </si>
-  <si>
-    <t>Burkholderia pseudomallei</t>
-  </si>
-  <si>
-    <t>28450</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Betaproteobacteria;Burkholderiales;Burkholderiaceae;Burkholderia</t>
-  </si>
-  <si>
-    <t>Haemophilus influenzae</t>
-  </si>
-  <si>
-    <t>727</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pasteurellales;Pasteurellaceae;Haemophilus</t>
-  </si>
-  <si>
-    <t>Providencia rettgeri</t>
-  </si>
-  <si>
-    <t>587</t>
-  </si>
-  <si>
-    <t>Pseudoalteromonas agarivorans</t>
-  </si>
-  <si>
-    <t>176102</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Alteromonadales;Pseudoalteromonadaceae;Pseudoalteromonas</t>
-  </si>
-  <si>
-    <t>Shigella dysenteriae</t>
-  </si>
-  <si>
-    <t>622</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Shigella</t>
-  </si>
-  <si>
-    <t>Yersinia pestis</t>
-  </si>
-  <si>
-    <t>632</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Yersiniaceae;Yersinia</t>
-  </si>
-  <si>
-    <t>2017-HCLON-0380</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>97.3799</t>
-  </si>
-  <si>
-    <t>99.1111</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1.74672</t>
-  </si>
-  <si>
-    <t>2017-SEQ-0905</t>
-  </si>
-  <si>
-    <t>Acinetobacter baumannii</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter</t>
-  </si>
-  <si>
-    <t>176</t>
-  </si>
-  <si>
-    <t>94.1176</t>
-  </si>
-  <si>
-    <t>95.6522</t>
-  </si>
-  <si>
-    <t>Acinetobacter calcoaceticus</t>
-  </si>
-  <si>
-    <t>471</t>
-  </si>
-  <si>
-    <t>2.13904</t>
-  </si>
-  <si>
-    <t>2.17391</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1.60428</t>
-  </si>
-  <si>
-    <t>Acinetobacter nosocomialis</t>
-  </si>
-  <si>
-    <t>106654</t>
-  </si>
-  <si>
-    <t>1.06952</t>
-  </si>
-  <si>
-    <t>1.08696</t>
-  </si>
-  <si>
-    <t>Acinetobacter pittii</t>
-  </si>
-  <si>
-    <t>48296</t>
-  </si>
-  <si>
-    <t>2017-SEQ-1501</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>96.6667</t>
-  </si>
-  <si>
-    <t>Enterococcus faecium</t>
-  </si>
-  <si>
-    <t>1352</t>
-  </si>
-  <si>
-    <t>Bacteria;Firmicutes;;;;Enterococcus</t>
-  </si>
-  <si>
-    <t>3.33333</t>
-  </si>
-  <si>
-    <t>2018-STH-0076</t>
-  </si>
-  <si>
-    <t>2016-SEQ-1221</t>
-  </si>
-  <si>
-    <t>Enterobacter hormaechei</t>
-  </si>
-  <si>
-    <t>158836</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Enterobacter</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>19.4444</t>
-  </si>
-  <si>
-    <t>20.8955</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>18.0556</t>
-  </si>
-  <si>
-    <t>19.403</t>
-  </si>
-  <si>
-    <t>Enterobacter cloacae</t>
-  </si>
-  <si>
-    <t>550</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>13.4328</t>
-  </si>
-  <si>
-    <t>Enterobacter asburiae</t>
-  </si>
-  <si>
-    <t>61645</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>11.1111</t>
-  </si>
-  <si>
-    <t>11.9403</t>
-  </si>
-  <si>
-    <t>8.33333</t>
-  </si>
-  <si>
-    <t>8.95522</t>
-  </si>
-  <si>
-    <t>Enterobacter roggenkampii</t>
-  </si>
-  <si>
-    <t>1812935</t>
-  </si>
-  <si>
-    <t>6.94444</t>
-  </si>
-  <si>
-    <t>7.46269</t>
-  </si>
-  <si>
-    <t>5.55556</t>
-  </si>
-  <si>
-    <t>5.97015</t>
-  </si>
-  <si>
-    <t>Enterobacter sp. HK169</t>
-  </si>
-  <si>
-    <t>1868135</t>
-  </si>
-  <si>
-    <t>4.16667</t>
-  </si>
-  <si>
-    <t>4.47761</t>
-  </si>
-  <si>
-    <t>Enterobacter ludwigii</t>
-  </si>
-  <si>
-    <t>299767</t>
-  </si>
-  <si>
-    <t>1.38889</t>
-  </si>
-  <si>
-    <t>1.49254</t>
-  </si>
-  <si>
-    <t>Enterobacter sp. Crenshaw</t>
-  </si>
-  <si>
-    <t>1977566</t>
-  </si>
-  <si>
-    <t>Klebsiella aerogenes</t>
-  </si>
-  <si>
-    <t>548</t>
-  </si>
-  <si>
-    <t>Lelliottia nimipressuralis</t>
-  </si>
-  <si>
-    <t>69220</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Lelliottia</t>
-  </si>
-  <si>
-    <t>2018-SEQ-0843</t>
-  </si>
-  <si>
-    <t>Vibrio parahaemolyticus</t>
-  </si>
-  <si>
-    <t>670</t>
-  </si>
-  <si>
-    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Vibrionales;Vibrionaceae;Vibrio</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>95.1613</t>
-  </si>
-  <si>
-    <t>98.3333</t>
-  </si>
-  <si>
-    <t>3.22581</t>
-  </si>
-  <si>
-    <t>Vibrio anguillarum</t>
-  </si>
-  <si>
-    <t>55601</t>
-  </si>
-  <si>
-    <t>1.6129</t>
-  </si>
-  <si>
-    <t>1.66667</t>
-  </si>
-  <si>
-    <t>2018-LET-0007</t>
-  </si>
-  <si>
-    <t>Campylobacter jejuni</t>
-  </si>
-  <si>
-    <t>197</t>
-  </si>
-  <si>
-    <t>Bacteria;;;;;Campylobacter</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>98.7654</t>
-  </si>
-  <si>
-    <t>Campylobacter coli</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
-    <t>1.23457</t>
-  </si>
-  <si>
-    <t>2018-STH-0255</t>
-  </si>
-  <si>
-    <t>Bacillus cereus</t>
-  </si>
-  <si>
-    <t>1396</t>
-  </si>
-  <si>
-    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Bacillaceae;Bacillus</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>64.2857</t>
-  </si>
-  <si>
-    <t>64.5933</t>
-  </si>
-  <si>
-    <t>Bacillus anthracis</t>
-  </si>
-  <si>
-    <t>1392</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>33.3333</t>
-  </si>
-  <si>
-    <t>33.4928</t>
-  </si>
-  <si>
-    <t>Bacillus thuringiensis</t>
-  </si>
-  <si>
-    <t>1428</t>
-  </si>
-  <si>
-    <t>1.90476</t>
-  </si>
-  <si>
-    <t>1.91388</t>
-  </si>
-  <si>
-    <t>2014-SEQ-0335</t>
-  </si>
-  <si>
-    <t>2019-SEQ-0183</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>85.2941</t>
-  </si>
-  <si>
-    <t>85.654</t>
-  </si>
-  <si>
-    <t>12.1849</t>
-  </si>
-  <si>
-    <t>12.2363</t>
-  </si>
-  <si>
-    <t>0.840336</t>
-  </si>
-  <si>
-    <t>0.843882</t>
+    <t>Serratia plymuthica</t>
+  </si>
+  <si>
+    <t>82996</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Yersiniaceae;Serratia</t>
   </si>
 </sst>
 </file>
@@ -1096,13 +1093,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="100.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -1149,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>4793471</v>
+        <v>4802782</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -1276,7 +1273,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="2">
-        <v>4716660</v>
+        <v>4716703</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>33</v>
@@ -1348,7 +1345,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="2">
-        <v>4001831</v>
+        <v>4003409</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -1374,7 +1371,7 @@
         <v>48</v>
       </c>
       <c r="E11" s="2">
-        <v>5096300</v>
+        <v>4906101</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>49</v>
@@ -1397,116 +1394,116 @@
         <v>48</v>
       </c>
       <c r="E12" s="2">
-        <v>1097202</v>
+        <v>1355124</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="2">
-        <v>23345</v>
+        <v>24309</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="2">
-        <v>141568</v>
+        <v>926</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="2">
-        <v>926</v>
+        <v>2577</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="2">
-        <v>2045</v>
+        <v>72349</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>48</v>
@@ -1518,10 +1515,10 @@
         <v>24</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1541,7 +1538,7 @@
         <v>24</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>26</v>
@@ -1549,51 +1546,51 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2737798</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2789846</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="B20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="2">
+        <v>191613</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="2">
-        <v>179487</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1610,10 +1607,10 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>26</v>
@@ -1621,36 +1618,36 @@
     </row>
     <row r="22" spans="1:8">
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E22" s="2">
-        <v>49540</v>
+        <v>53049</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="E23" s="2">
         <v>209484</v>
@@ -1659,10 +1656,10 @@
         <v>36</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1682,10 +1679,10 @@
         <v>36</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1696,56 +1693,56 @@
         <v>99</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E25" s="2">
-        <v>18392</v>
+        <v>2416</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="E26" s="2">
-        <v>10158</v>
+        <v>58416</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E27" s="2">
-        <v>58416</v>
+        <v>24890</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>24</v>
@@ -1759,16 +1756,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="2" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="E28" s="2">
-        <v>24890</v>
+        <v>6649</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>24</v>
@@ -1811,10 +1808,10 @@
         <v>112</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E30" s="2">
-        <v>1785</v>
+        <v>17761</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>24</v>
@@ -1896,124 +1893,124 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="2">
+        <v>45156</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="2">
-        <v>5288405</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H34" s="2" t="s">
+      <c r="E35" s="2">
+        <v>5287846</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" s="2" t="s">
+      <c r="G35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E36" s="2">
         <v>0</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" s="2" t="s">
+      <c r="F36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" s="2" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="2">
-        <v>3918535</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="E37" s="2">
+        <v>3919197</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="2">
-        <v>4431</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="B38" s="2" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="E38" s="2">
-        <v>0</v>
+        <v>8586</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2024,13 +2021,13 @@
         <v>142</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E39" s="2">
-        <v>3289</v>
+        <v>5127</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>143</v>
@@ -2041,30 +2038,30 @@
     </row>
     <row r="40" spans="1:8">
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>23</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="E40" s="2">
-        <v>3892</v>
+        <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>143</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>16</v>
@@ -2079,24 +2076,24 @@
         <v>3016528</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="E42" s="2">
         <v>754</v>
@@ -2105,81 +2102,99 @@
         <v>24</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="D43" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="2">
+        <v>3182418</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="B44" s="2" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="2">
+        <v>152299</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="2">
-        <v>1902398</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="E45" s="2">
-        <v>64323</v>
+        <v>932897</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="B46" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E46" s="2">
-        <v>354449</v>
+        <v>4678</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>168</v>
@@ -2190,525 +2205,600 @@
     </row>
     <row r="47" spans="1:8">
       <c r="B47" s="2" t="s">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="E47" s="2">
-        <v>1850469</v>
+        <v>76654</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="B48" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E48" s="2">
-        <v>78305</v>
+        <v>0</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E49" s="2">
-        <v>3125</v>
+        <v>1773</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E50" s="2">
-        <v>0</v>
+        <v>189432</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="2" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="E51" s="2">
-        <v>189432</v>
+        <v>201160</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E52" s="2">
-        <v>9189</v>
+        <v>207</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>139</v>
+        <v>24</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="E53" s="2">
-        <v>201160</v>
+        <v>232</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:8">
+      <c r="A54" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="B54" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="E54" s="2">
-        <v>1803</v>
+        <v>5094690</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="2" t="s">
-        <v>193</v>
+        <v>23</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>194</v>
+        <v>23</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="E55" s="2">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>189</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>190</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="B56" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E56" s="2">
-        <v>540</v>
+        <v>16154</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:8">
+      <c r="A57" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>119</v>
+        <v>195</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="E57" s="2">
-        <v>86325</v>
+        <v>1727682</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>24</v>
+        <v>198</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>189</v>
+        <v>14</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>190</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E58" s="2">
-        <v>5094690</v>
+        <v>3653505</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="B59" s="2" t="s">
-        <v>23</v>
+        <v>206</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>23</v>
+        <v>207</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="E59" s="2">
-        <v>0</v>
+        <v>1472779</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="B60" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E60" s="2">
-        <v>16154</v>
+        <v>68844</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E61" s="2">
-        <v>1715091</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G61" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>215</v>
-      </c>
     </row>
     <row r="62" spans="1:8">
+      <c r="A62" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="B62" s="2" t="s">
-        <v>216</v>
+        <v>9</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2">
+        <v>692141</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E62" s="2">
-        <v>12591</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>218</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="B63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="2">
+        <v>2983937</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E63" s="2">
-        <v>3586033</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="B64" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="2">
+        <v>3326</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E65" s="2">
+        <v>4724985</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E64" s="2">
-        <v>1540251</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="H65" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="B66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="E66" s="2">
+        <v>15203</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="B65" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E65" s="2">
-        <v>68844</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="2" t="s">
-        <v>235</v>
+      <c r="H66" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>9</v>
+        <v>231</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>10</v>
+        <v>232</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="E67" s="2">
-        <v>694771</v>
+        <v>4429632</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>237</v>
+        <v>76</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="B68" s="2" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="E68" s="2">
-        <v>2983949</v>
+        <v>202199</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="B69" s="2" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="E69" s="2">
-        <v>3550</v>
+        <v>12173</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="B70" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="2">
+        <v>25744</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="B71" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>243</v>
+      <c r="E71" s="2">
+        <v>336</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="B72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>